<commit_message>
Added and updated values
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thimo Merke\Documents\carbon-removal-technologies-potential-cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB214142-4DFD-4520-9FDD-20780115D0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EFC4057-6CD9-4667-96BA-341239222DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="38385" windowHeight="18435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5025" yWindow="1620" windowWidth="38385" windowHeight="18435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="76">
   <si>
     <t>Technology</t>
   </si>
@@ -231,6 +232,39 @@
   </si>
   <si>
     <t>land, water, fertilizer</t>
+  </si>
+  <si>
+    <t>42 - 300 (Avg.: 147)</t>
+  </si>
+  <si>
+    <t>0.3 - 12 (Avg.: 5.4)</t>
+  </si>
+  <si>
+    <t>land required, fertilization, processing, construction of bioenergy plants</t>
+  </si>
+  <si>
+    <t>none (doesn't block land use)</t>
+  </si>
+  <si>
+    <t>medium, possibly high competition for land</t>
+  </si>
+  <si>
+    <t>can be used with agroforestry</t>
+  </si>
+  <si>
+    <t>improved soil quality, reduced land erosion</t>
+  </si>
+  <si>
+    <t>possible high competition for land, threat for food security</t>
+  </si>
+  <si>
+    <t>electricity production, displacement of fossil fuels</t>
+  </si>
+  <si>
+    <t>phytoplankton can increase oxygen content of oceans</t>
+  </si>
+  <si>
+    <t>can improve soil fertility, reduce ocean acidity</t>
   </si>
 </sst>
 </file>
@@ -559,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,4 +869,327 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5FEDB9-B209-4CE4-9576-2BE683F2B089}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>